<commit_message>
Added ability to delete past words through context menu Fixed few bugs with personalization Added tooltips to buttons and comboboxes
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -427,14 +427,14 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="114" customWidth="1"/>
-    <col min="3" max="3" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -483,11 +483,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -508,11 +508,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added bug, removed .suo from tracking
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Priority</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Stores the user settings using VisualStudio built-in settings file</t>
+  </si>
+  <si>
+    <t>Doesn't work well when invoking from PDF highlighted word</t>
+  </si>
+  <si>
+    <t>Create installation project</t>
   </si>
 </sst>
 </file>
@@ -133,6 +139,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -180,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,7 +224,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -467,13 +476,12 @@
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -492,44 +500,61 @@
       </c>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>2</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C10">
-    <sortCondition ref="A2:A10"/>
+  <sortState ref="A2:C12">
+    <sortCondition ref="A2:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added change to support ClickOnce deployment
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,27 +487,29 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -515,17 +517,18 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>1</v>
+      <c r="A9" s="3">
+        <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -564,7 +567,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD13">
+  <sortState ref="A2:C13">
     <sortCondition ref="A2:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added list of potential hotkey combinations to try registering as activation shortcut for the application. Moved all hard-coded strings into resources for later localization efforts. Updated code to refer to ProductName and CompanyName of the assembly instead of using hard-coded names.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Priority</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>Add a review feature to let users review words they have learned</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added a list of pre-defined shortcut keys and attempt to register each one </t>
+  </si>
+  <si>
+    <t>Use ClickOnce to deploy</t>
+  </si>
+  <si>
+    <t>Add ability to deploy ClickOnce without hardcoding publisher name and product name</t>
   </si>
 </sst>
 </file>
@@ -451,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +474,7 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="110.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="90.5703125" customWidth="1"/>
+    <col min="4" max="4" width="68.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -474,6 +487,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -520,11 +536,14 @@
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,14 +582,16 @@
       </c>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12"/>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -581,11 +602,11 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>2</v>
-      </c>
-      <c r="B14" s="7" t="s">
+    <row r="14" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -615,18 +636,26 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD18">
-    <sortCondition ref="A2:A18"/>
+  <sortState ref="A2:D19">
+    <sortCondition ref="A2:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added restore settings option in configuration form. Redesigned some layout on config form. Fixed bugs: removing inactive site allows further deleting the only site left.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Priority</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Add ability for users to speak a word, or a sentence and process using speech recognition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look at hooking up Bing translator API or Google translator API. Bing offers free 2m characters a month, Google doesn't </t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -193,6 +196,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,11 +614,11 @@
       <c r="C9" s="9"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -742,20 +749,30 @@
       </c>
     </row>
     <row r="24" spans="1:4" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
         <v>3</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D25" s="9"/>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD24">
-    <sortCondition ref="A2:A24"/>
+  <sortState ref="A2:D25">
+    <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added code to mark default translation sites as required so users can't delete them. This change seems to work, not tested thoroughly yet. Also updated bug list.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Priority</t>
   </si>
@@ -112,6 +112,13 @@
   </si>
   <si>
     <t>Let the WebBrowser control lazy-load so the pop up form doesn't take too long to display</t>
+  </si>
+  <si>
+    <t>Needed Application.DoEvents before pasting</t>
+  </si>
+  <si>
+    <t>Changed control to use Url property instead of manually setting a static HTML content. Also  
+control was previously using older IE versions to browse web.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +517,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +525,7 @@
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="110.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="79.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -576,10 +583,10 @@
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="11"/>
@@ -625,15 +632,17 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>2</v>
-      </c>
-      <c r="B11" s="11" t="s">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
@@ -761,12 +770,15 @@
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>2</v>
-      </c>
-      <c r="B25" s="9" t="s">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>2</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>31</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the past word control to be just button for more solid behavior
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Priority</t>
   </si>
@@ -131,6 +131,13 @@
   </si>
   <si>
     <t>Prevent the config form from being resized</t>
+  </si>
+  <si>
+    <t>Change the minimum size for the translation window</t>
+  </si>
+  <si>
+    <t>Sometimes the app crashes after translation window is closed. Probably related to there being two webbrowser controls?
+Attempted to read or write protected memory. This is often an indication that other memory is corrupt.</t>
   </si>
 </sst>
 </file>
@@ -526,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +843,22 @@
         <v>3</v>
       </c>
       <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>2</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>2</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:D30">

</xml_diff>

<commit_message>
Prevented config form from being resized. Changed the minimum size for the translation window
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Priority</t>
   </si>
@@ -138,6 +138,9 @@
   <si>
     <t>Sometimes the app crashes after translation window is closed. Probably related to there being two webbrowser controls?
 Attempted to read or write protected memory. This is often an indication that other memory is corrupt.</t>
+  </si>
+  <si>
+    <t>Changed the way to add new site. Instead of using calibrate words, let users choose any word and then ask them for it</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,10 +804,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>2</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="13">
+        <v>2</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -825,44 +828,52 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>2</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="13">
+        <v>2</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>2</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>2</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
         <v>3</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B32" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>2</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>2</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>39</v>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>2</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D30">
-    <sortCondition ref="A2:A30"/>
+  <sortState ref="A2:D32">
+    <sortCondition ref="A2:A32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed method of adding new site. Now allowing users to add any random word. However, this change doesn't work with Unicode letters yet.
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Priority</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Changed the way to add new site. Instead of using calibrate words, let users choose any word and then ask them for it</t>
+  </si>
+  <si>
+    <t>Prevent popup from the webbrowser control</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +872,14 @@
       </c>
       <c r="B33" s="9" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>1</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>